<commit_message>
Activity+new jon TAS Job Type
</commit_message>
<xml_diff>
--- a/TestData/T1432_OpportunityToEngagementConversionMappingForFASJobTypes.xlsx
+++ b/TestData/T1432_OpportunityToEngagementConversionMappingForFASJobTypes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VKumar0427\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3BD45F-0E06-4E27-9BFD-A72299CB4050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1888341F-E970-495D-9AE9-8517E0D6F649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="-120" yWindow="-120" windowWidth="28800" windowHeight="14520" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView showHorizontalScroll="0" showVerticalScroll="0" xWindow="-120" yWindow="-120" windowWidth="28950" windowHeight="14640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddOpportunity" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="86">
   <si>
     <t>Client</t>
   </si>
@@ -280,6 +280,12 @@
   </si>
   <si>
     <t>CVAS - IP Valuation</t>
+  </si>
+  <si>
+    <t>TAS - ESG Due Diligence &amp; Analytics</t>
+  </si>
+  <si>
+    <t>TAS - Due Diligence Services</t>
   </si>
 </sst>
 </file>
@@ -1060,10 +1066,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD12"/>
+  <dimension ref="A1:AD13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C12"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2165,6 +2171,95 @@
         <v>77</v>
       </c>
     </row>
+    <row r="13" spans="1:30" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="L13" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N13" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R13" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="S13" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="T13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="U13" t="s">
+        <v>30</v>
+      </c>
+      <c r="V13" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="W13" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="X13" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y13" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z13" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA13" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB13" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>77</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2211,7 +2306,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H2"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2284,16 +2379,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
     <col min="4" max="5" width="38" bestFit="1" customWidth="1"/>
   </cols>
@@ -2496,6 +2591,17 @@
         <v>83</v>
       </c>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>